<commit_message>
Services in single and multiple shipments
</commit_message>
<xml_diff>
--- a/Template/Template.xlsx
+++ b/Template/Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omerm\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ABS\ABS System\ABS-System-Backend\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0E70A01-0334-49EE-9D7C-F6C97B8D27AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{44D00D9F-BD3C-4F36-AC3A-491061D8B145}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <definedName name="DeliveryExchange">"{""Delivery"",1;""Exchange"",2}"</definedName>
     <definedName name="lookup_list">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,8 +27,90 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Adham Ahmed</author>
+  </authors>
+  <commentList>
+    <comment ref="T1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adham Ahmed:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
++5 EGP will be added on the fees, if you don't choose Yes or No, the services you chose while registration will be applied</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adham Ahmed:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
++10 EGP will be added on the fees, if you don't choose Yes or No, the services you chose while registration will be applied</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Adham Ahmed:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
++15 EGP will be added on the fees, if you don't choose Yes or No, the services you chose while registration will be applied</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Ref</t>
   </si>
@@ -79,9 +160,6 @@
     <t>latitude</t>
   </si>
   <si>
-    <t>Product</t>
-  </si>
-  <si>
     <t>PackageType</t>
   </si>
   <si>
@@ -89,16 +167,25 @@
   </si>
   <si>
     <t>Service</t>
+  </si>
+  <si>
+    <t>allowOpenPackages</t>
+  </si>
+  <si>
+    <t>sameDayDelivery</t>
+  </si>
+  <si>
+    <t>feesOnConsignee</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +200,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -455,111 +555,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD15E65C-5D97-4288-8C15-7E06D2500A20}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.77734375" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.6640625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" customWidth="1"/>
-    <col min="19" max="20" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="10" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15.5546875" customWidth="1"/>
+    <col min="18" max="19" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>15</v>
+      <c r="U1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{BF833203-ECF4-42F5-8BEC-CF9183BAB622}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
       <formula1>"Delivery,Return,Exchange"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{E927A4D1-CEE7-4135-9FDE-52E94E9ECC7A}">
-      <formula1>"COD,Bulk Mail"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{19978039-342B-449F-83E8-A8F818DDFAA6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>"Parcel,Document,Bulk"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q1048576" xr:uid="{70CF2512-C9EC-4C1F-BA68-52B428CF12B1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P1048576">
       <formula1>"Dokki,Giza,October,Maadi"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:V1048576">
+      <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>